<commit_message>
ms office excel can not open bug fixed
</commit_message>
<xml_diff>
--- a/examples/complex.xlsx
+++ b/examples/complex.xlsx
@@ -6,10 +6,10 @@
   <bookViews>
     <workbookView showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="204" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
-  <calcPr iterateCount="100" iterate="0" iterateDelta="0.001" refMode="A1"/>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1" state="visible"/>
   </sheets>
+  <calcPr iterateCount="100" iterate="0" iterateDelta="0.001" refMode="A1"/>
 </workbook>
 </file>
 
@@ -59,6 +59,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="$#,##0.00"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="12"/>
@@ -295,9 +298,6 @@
       <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="$#,##0.00"/>
-  </numFmts>
 </styleSheet>
 </file>
 
@@ -626,20 +626,13 @@
   <sheetPr filterMode="0">
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.85" defaultColWidth="0"/>
-  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="1" usePrinterDefaults="0" verticalDpi="300"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-  <dimension ref="A1:D10"/>
+  <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
     <col min="1" max="1" hidden="0" width="20" customWidth="1" collapsed="0" outlineLevel="0" style="1"/>
     <col min="2" max="2" hidden="0" width="20" customWidth="1" collapsed="0" outlineLevel="0" style="1"/>
@@ -797,5 +790,12 @@
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="1" usePrinterDefaults="0" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>